<commit_message>
Add config.yaml, multi-period OOS, CVaR/MaxDD constraints, optimization doc
</commit_message>
<xml_diff>
--- a/metrics_comparison.xlsx
+++ b/metrics_comparison.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5921624985872886</v>
+        <v>1.017517448585473</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5951154482475125</v>
+        <v>0.4223807153183843</v>
       </c>
       <c r="D2" t="n">
-        <v>0.274864555116162</v>
+        <v>0.2446916143694868</v>
       </c>
       <c r="E2" t="n">
-        <v>2.05597789066941</v>
+        <v>1.60357238366937</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.1019048478251513</v>
+        <v>-0.1128288494190266</v>
       </c>
       <c r="G2" t="n">
-        <v>0.645658444999943</v>
+        <v>0.564231488800237</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9882576971199195</v>
+        <v>1.676451378490478</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9937091707602768</v>
+        <v>0.6391979074220058</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2751775649069436</v>
+        <v>0.2445720448915195</v>
       </c>
       <c r="E3" t="n">
-        <v>3.502135688591375</v>
+        <v>2.490873017364748</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.1020461619825004</v>
+        <v>-0.1127528199373788</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6464121558574881</v>
+        <v>0.5639702106451753</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4761099218206262</v>
+        <v>0.8448534768133353</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4784017878639031</v>
+        <v>0.3599118058759405</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2399162509686279</v>
+        <v>0.2127515357305201</v>
       </c>
       <c r="E4" t="n">
-        <v>1.868992975896982</v>
+        <v>1.550690596630148</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.08843266528217224</v>
+        <v>-0.09281505800686342</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5689179502129542</v>
+        <v>0.4989226723653052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>